<commit_message>
icones login e doc atualizada
</commit_message>
<xml_diff>
--- a/Documentação/Sprint Backlog/Sprint Backlog v1.xlsx
+++ b/Documentação/Sprint Backlog/Sprint Backlog v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valemobibr-my.sharepoint.com/personal/vinicius_cano_valemobi_com_br/Documents/Documentos/ads3/grupoPi3Semestre/Documentação/Sprint Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDAB6A1E-9465-4B45-9483-2E76252CEBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{CDAB6A1E-9465-4B45-9483-2E76252CEBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A4CE942-9AC9-4F7B-B7BD-CB8B3353C7B0}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{8E247AC1-F5EC-47B9-AF03-9EBFD3B9FE4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8E247AC1-F5EC-47B9-AF03-9EBFD3B9FE4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Site" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>Home</t>
   </si>
@@ -197,6 +197,63 @@
   </si>
   <si>
     <t>Botão para ele poder confirmar seu cadastro</t>
+  </si>
+  <si>
+    <t>Cards infromando os valores atuais do usuario</t>
+  </si>
+  <si>
+    <t>Gráficos com as despesas e receitas do usuário</t>
+  </si>
+  <si>
+    <t>Modal para inclusão de novas despesas/receitas</t>
+  </si>
+  <si>
+    <t>Menu lateral para acesso as outras áreas exclusivas do usuário</t>
+  </si>
+  <si>
+    <t>Cadastro dos carros do cliente</t>
+  </si>
+  <si>
+    <t>Cadastrar o tipo, modelo, marca, placa e dono do veículo</t>
+  </si>
+  <si>
+    <t>Página para mostrar detalhadamente as despesas / receitas do usuário</t>
+  </si>
+  <si>
+    <t>Mostrar a descrição, valor, placa e categoria de receitas / despesas</t>
+  </si>
+  <si>
+    <t>Filtro para usuário selecionar por cliente, valor ou placa</t>
+  </si>
+  <si>
+    <t>Preencher a descrição da transação</t>
+  </si>
+  <si>
+    <t>Preencher o valor da transação</t>
+  </si>
+  <si>
+    <t>Selecionar se é uma Entrada (receita) ou saída (despesa)</t>
+  </si>
+  <si>
+    <t>Selecionar a categoria da transação</t>
+  </si>
+  <si>
+    <t>Preencher o nome do cliente</t>
+  </si>
+  <si>
+    <t>Preencher a placa do carro do cliente</t>
+  </si>
+  <si>
+    <t>Possibilitar o usuário a trocar a foto de perfil</t>
+  </si>
+  <si>
+    <t>Possibilitar o usuário a trocar seu e-mail</t>
+  </si>
+  <si>
+    <t>Possibilitar o usuário a atualizar o nome da oficina</t>
+  </si>
+  <si>
+    <t>Possibilitar o usuário a atualizar o CNPJ da oficina</t>
   </si>
 </sst>
 </file>
@@ -464,58 +521,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -524,12 +587,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530B6C52-7D5E-4DAB-A716-D1125F56B837}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:G19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,537 +930,591 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:11" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="18" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="17" t="s">
+      <c r="J2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="22"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="G3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="22"/>
+    </row>
+    <row r="4" spans="1:11" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="E4" s="11"/>
+      <c r="C4" s="22"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="G4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="E5" s="11"/>
+      <c r="C5" s="22"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="G5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="E6" s="13"/>
+      <c r="C6" s="22"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="I6" s="10"/>
+      <c r="G6" s="26"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="1:11" s="7" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="E7" s="7" t="s">
+      <c r="C7" s="23"/>
+      <c r="E7" s="24" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="26"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="I8" s="9" t="s">
+      <c r="G8" s="25"/>
+      <c r="I8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="17" t="s">
+      <c r="J8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
       <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="22"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="18"/>
-    </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="G9" s="25"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="22"/>
+    </row>
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="22"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="18"/>
-    </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="G10" s="25"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="E11" s="10"/>
+      <c r="C11" s="22"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="18"/>
-    </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="G11" s="25"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="22"/>
+    </row>
+    <row r="12" spans="1:11" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="E12" s="12"/>
+      <c r="C12" s="22"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="18"/>
-    </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="G12" s="26"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="E13" s="25" t="s">
+      <c r="C13" s="23"/>
+      <c r="E13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="24" t="s">
+      <c r="E14" s="28"/>
+      <c r="F14" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="I14" s="9" t="s">
+      <c r="G14" s="25"/>
+      <c r="I14" s="18" t="s">
         <v>25</v>
       </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
       <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="24" t="s">
+      <c r="C15" s="25"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="I15" s="11"/>
+      <c r="G15" s="25"/>
+      <c r="I15" s="19"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="K15" s="22"/>
+    </row>
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="24" t="s">
+      <c r="C16" s="25"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="18"/>
-    </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="G16" s="25"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="24" t="s">
+      <c r="C17" s="25"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="18"/>
-    </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="22" t="s">
+      <c r="G17" s="25"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="1:11" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26"/>
+      <c r="B18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="E18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="I18" s="11"/>
+      <c r="G18" s="25"/>
+      <c r="I18" s="19"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="1:11" s="8" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28" t="s">
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:11" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="I19" s="13"/>
+      <c r="G19" s="26"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:11" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14"/>
-      <c r="E20" s="9" t="s">
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" s="7" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="17" t="s">
+      <c r="J20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="E21" s="11"/>
+    <row r="21" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="18"/>
-    </row>
-    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14"/>
-      <c r="E22" s="11"/>
+      <c r="G21" s="22"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="22"/>
+    </row>
+    <row r="22" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="18"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="18"/>
-    </row>
-    <row r="23" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14"/>
-      <c r="E23" s="11"/>
+      <c r="G22" s="22"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="22"/>
+    </row>
+    <row r="23" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="18"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="18"/>
-    </row>
-    <row r="24" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="14"/>
-      <c r="E24" s="11"/>
+      <c r="G23" s="22"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="22"/>
+    </row>
+    <row r="24" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="I24" s="11"/>
+      <c r="G24" s="22"/>
+      <c r="I24" s="19"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="18"/>
-    </row>
-    <row r="25" spans="1:11" s="8" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="14"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="29" t="s">
+      <c r="K24" s="22"/>
+    </row>
+    <row r="25" spans="1:11" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="8"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="I25" s="13"/>
+      <c r="G25" s="23"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="14"/>
-      <c r="E26" s="16"/>
-      <c r="I26" s="9" t="s">
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="8"/>
+      <c r="E26" s="10"/>
+      <c r="I26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="17" t="s">
+      <c r="J26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
-      <c r="E27" s="16"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="18"/>
-    </row>
-    <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="14"/>
-      <c r="E28" s="16"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="18"/>
-    </row>
-    <row r="29" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="14"/>
-      <c r="E29" s="16"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="18"/>
-    </row>
-    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="14"/>
-      <c r="E30" s="16"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="18"/>
-    </row>
-    <row r="31" spans="1:11" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="14"/>
-      <c r="E31" s="16"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="19"/>
-    </row>
-    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="14"/>
-      <c r="E32" s="16"/>
-      <c r="I32" s="9" t="s">
+    <row r="27" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="8"/>
+      <c r="E27" s="10"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K27" s="22"/>
+    </row>
+    <row r="28" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="8"/>
+      <c r="E28" s="10"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" s="22"/>
+    </row>
+    <row r="29" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="8"/>
+      <c r="E29" s="10"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K29" s="22"/>
+    </row>
+    <row r="30" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="E30" s="10"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="E31" s="10"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="23"/>
+    </row>
+    <row r="32" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="E32" s="10"/>
+      <c r="I32" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="17" t="s">
+      <c r="J32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="14"/>
-      <c r="E33" s="16"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="18"/>
-    </row>
-    <row r="34" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="14"/>
-      <c r="E34" s="16"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="18"/>
-    </row>
-    <row r="35" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="14"/>
-      <c r="E35" s="16"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="18"/>
-    </row>
-    <row r="36" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="14"/>
-      <c r="E36" s="16"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="18"/>
-    </row>
-    <row r="37" spans="1:11" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="E33" s="10"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="E34" s="10"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="E35" s="10"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K35" s="22"/>
+    </row>
+    <row r="36" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="E36" s="10"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" s="22"/>
+    </row>
+    <row r="37" spans="1:11" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="15"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="1"/>
-      <c r="E37" s="16"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="19"/>
-    </row>
-    <row r="38" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="10"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K37" s="23"/>
+    </row>
+    <row r="38" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
@@ -1413,32 +1524,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="G7:G12"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="K2:K7"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="I14:I19"/>
+    <mergeCell ref="K14:K19"/>
+    <mergeCell ref="I20:I25"/>
+    <mergeCell ref="K20:K25"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="K26:K31"/>
+    <mergeCell ref="I32:I37"/>
+    <mergeCell ref="K32:K37"/>
     <mergeCell ref="E20:E25"/>
     <mergeCell ref="G20:G25"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="E13:E19"/>
     <mergeCell ref="G13:G19"/>
-    <mergeCell ref="I20:I25"/>
-    <mergeCell ref="K20:K25"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="K26:K31"/>
-    <mergeCell ref="I32:I37"/>
-    <mergeCell ref="K32:K37"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="K2:K7"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="I14:I19"/>
-    <mergeCell ref="K14:K19"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="G7:G12"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="G2:G6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>